<commit_message>
Finish up blog content.
</commit_message>
<xml_diff>
--- a/content/blog/2022-01-22-Clean-Lipid-Names-1/Annotation.xlsx
+++ b/content/blog/2022-01-22-Clean-Lipid-Names-1/Annotation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\jaunty-blogdown\content\blog\2022-01-22-Clean-Lipid-Names-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB8B335-1CC1-46BD-AB34-84129F59AEF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02637DE-B6E0-4634-80F8-0236B4C66524}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6210" windowHeight="6855" xr2:uid="{B782973C-B63B-45B9-946A-0EAA227300F5}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>Transition_Name</t>
-  </si>
-  <si>
     <t>Precursor Ion</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>LPC 17:1 (c)</t>
+  </si>
+  <si>
+    <t>Given Name</t>
   </si>
 </sst>
 </file>
@@ -133,7 +133,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B09E4E23-22DF-4B8F-B7CA-9703E38204D8}" name="Table1" displayName="Table1" ref="A1:C11" totalsRowShown="0">
   <autoFilter ref="A1:C11" xr:uid="{669A7E1D-CE01-460F-BEEE-29991D990823}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E20B83F1-A6D6-415B-B9BE-E6C771F7CCB4}" name="Transition_Name"/>
+    <tableColumn id="1" xr3:uid="{E20B83F1-A6D6-415B-B9BE-E6C771F7CCB4}" name="Given Name"/>
     <tableColumn id="3" xr3:uid="{607B8EFF-0F6B-4FEA-AD5A-123FB2D3032A}" name="Precursor Ion"/>
     <tableColumn id="4" xr3:uid="{63E1BC41-950B-4B1D-AA22-0B69814E8100}" name="Product Ion" dataDxfId="0"/>
   </tableColumns>
@@ -442,7 +442,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,18 +456,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>454.3</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>454.3</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>454.3</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>487.4</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>487.4</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>487.4</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>508.3</v>
@@ -544,7 +544,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>508.3</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>508.3</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1">
         <v>508.3</v>

</xml_diff>